<commit_message>
byly upraveny průěmrné dodávky a upraven app.py
# Conflicts:
#	app.py
</commit_message>
<xml_diff>
--- a/prumerna_dodavka_tepla.xlsx
+++ b/prumerna_dodavka_tepla.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cezdata-my.sharepoint.com/personal/michal_pekarek01_cez_cz/Documents/Plocha/práce/#30 Prediktivní model EPRU/github/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cezdata-my.sharepoint.com/personal/michal_pekarek01_cez_cz/Documents/Plocha/práce/#30 Prediktivní model EPRU/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="11_8A8D061F5CD9D40F3AFE31D2F8F2D3C274D93BF9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D73D0EA4-4162-4B0C-B0E1-8BE42C1CBA99}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_2B8B061F6721173CF2FE31D2F8F2D3C2C4DC5C93" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5EF6A76-7934-46AF-8173-829CBA01766F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -401,8 +401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
-      <selection activeCell="D268" sqref="D268"/>
+    <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
+      <selection activeCell="C276" sqref="C276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,7 +426,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>224.3324731182675</v>
+        <v>222.99319783198251</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -437,7 +437,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>226.40967741936839</v>
+        <v>224.74543010752731</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -448,7 +448,7 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>229.04516129026331</v>
+        <v>226.91602150534561</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -459,7 +459,7 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>249.35322580651771</v>
+        <v>248.31972899733611</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -470,7 +470,7 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>253.21451612902169</v>
+        <v>257.20956639565361</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -481,7 +481,7 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>256.64999999996701</v>
+        <v>261.2523848238298</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -492,7 +492,7 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>259.03870967744041</v>
+        <v>263.16463414635137</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -503,7 +503,7 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>261.83709677424088</v>
+        <v>268.07755376347632</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -514,7 +514,7 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>249.01935483869391</v>
+        <v>258.90567204298861</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -525,7 +525,7 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>237.9274193548124</v>
+        <v>247.42571815717289</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -536,7 +536,7 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>229.69193548386571</v>
+        <v>240.19826558265339</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -547,7 +547,7 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>223.91290322575909</v>
+        <v>233.4906048386857</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -558,7 +558,7 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>220.0322580645537</v>
+        <v>228.65625000002021</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -569,7 +569,7 @@
         <v>13</v>
       </c>
       <c r="C15">
-        <v>221.87419354839389</v>
+        <v>229.67361617577899</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -580,7 +580,7 @@
         <v>14</v>
       </c>
       <c r="C16">
-        <v>227.7999999999752</v>
+        <v>234.97216339411389</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -591,7 +591,7 @@
         <v>15</v>
       </c>
       <c r="C17">
-        <v>239.64677419358739</v>
+        <v>245.59354838710269</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -602,7 +602,7 @@
         <v>16</v>
       </c>
       <c r="C18">
-        <v>252.23387096771941</v>
+        <v>256.01865591397723</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -613,7 +613,7 @@
         <v>17</v>
       </c>
       <c r="C19">
-        <v>259.03870967743279</v>
+        <v>261.50862903225828</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -624,7 +624,7 @@
         <v>18</v>
       </c>
       <c r="C20">
-        <v>263.09838709675319</v>
+        <v>265.24615591396503</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -635,7 +635,7 @@
         <v>19</v>
       </c>
       <c r="C21">
-        <v>261.29354838709219</v>
+        <v>262.19021505376338</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -646,7 +646,7 @@
         <v>20</v>
       </c>
       <c r="C22">
-        <v>244.30000000000899</v>
+        <v>246.32831978319879</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -657,7 +657,7 @@
         <v>21</v>
       </c>
       <c r="C23">
-        <v>235.3467741935859</v>
+        <v>233.14336043363201</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -668,7 +668,7 @@
         <v>22</v>
       </c>
       <c r="C24">
-        <v>227.8112903225626</v>
+        <v>227.74572580642351</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -679,7 +679,7 @@
         <v>23</v>
       </c>
       <c r="C25">
-        <v>221.8161290322671</v>
+        <v>220.91263440860789</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -690,7 +690,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <v>196.91403508772089</v>
+        <v>213.65502976189501</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -701,7 +701,7 @@
         <v>1</v>
       </c>
       <c r="C27">
-        <v>199.63684210527211</v>
+        <v>217.5491369047694</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -712,7 +712,7 @@
         <v>2</v>
       </c>
       <c r="C28">
-        <v>202.222807017539</v>
+        <v>221.63309523809119</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -723,7 +723,7 @@
         <v>3</v>
       </c>
       <c r="C29">
-        <v>225.24464285711289</v>
+        <v>240.3453571428436</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -734,7 +734,7 @@
         <v>4</v>
       </c>
       <c r="C30">
-        <v>227.4947368421208</v>
+        <v>248.64002949852579</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -745,7 +745,7 @@
         <v>5</v>
       </c>
       <c r="C31">
-        <v>229.0298245614068</v>
+        <v>253.02179941005201</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -756,7 +756,7 @@
         <v>6</v>
       </c>
       <c r="C32">
-        <v>229.3017543859396</v>
+        <v>255.0911209439175</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -767,7 +767,7 @@
         <v>7</v>
       </c>
       <c r="C33">
-        <v>224.72105263158869</v>
+        <v>249.20262536874799</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -778,7 +778,7 @@
         <v>8</v>
       </c>
       <c r="C34">
-        <v>211.05438596490171</v>
+        <v>233.2724188790441</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -789,7 +789,7 @@
         <v>9</v>
       </c>
       <c r="C35">
-        <v>198.96842105267979</v>
+        <v>219.57252423096119</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -800,7 +800,7 @@
         <v>10</v>
       </c>
       <c r="C36">
-        <v>192.0596491228095</v>
+        <v>211.19485040033129</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -811,7 +811,7 @@
         <v>11</v>
       </c>
       <c r="C37">
-        <v>186.68421052629131</v>
+        <v>205.54772861356551</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -822,7 +822,7 @@
         <v>12</v>
       </c>
       <c r="C38">
-        <v>182.95614035089349</v>
+        <v>198.99179941002981</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -833,7 +833,7 @@
         <v>13</v>
       </c>
       <c r="C39">
-        <v>183.73508771927621</v>
+        <v>198.17165572366281</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -844,7 +844,7 @@
         <v>14</v>
       </c>
       <c r="C40">
-        <v>187.6210526316018</v>
+        <v>201.73987344181549</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -855,7 +855,7 @@
         <v>15</v>
       </c>
       <c r="C41">
-        <v>197.85087719301509</v>
+        <v>212.4400342563641</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -866,7 +866,7 @@
         <v>16</v>
       </c>
       <c r="C42">
-        <v>215.82280701748499</v>
+        <v>230.45805309731591</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -877,7 +877,7 @@
         <v>17</v>
       </c>
       <c r="C43">
-        <v>230.39649122807589</v>
+        <v>244.08902654867461</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -888,7 +888,7 @@
         <v>18</v>
       </c>
       <c r="C44">
-        <v>236.12280701755199</v>
+        <v>249.17203539822131</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -899,7 +899,7 @@
         <v>19</v>
       </c>
       <c r="C45">
-        <v>232.86315789469111</v>
+        <v>245.8559292035257</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -910,7 +910,7 @@
         <v>20</v>
       </c>
       <c r="C46">
-        <v>216.80877192988339</v>
+        <v>231.96457227142949</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -921,7 +921,7 @@
         <v>21</v>
       </c>
       <c r="C47">
-        <v>212.45964912278171</v>
+        <v>221.35834808257439</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -932,7 +932,7 @@
         <v>22</v>
       </c>
       <c r="C48">
-        <v>204.5438596491187</v>
+        <v>216.38112094395419</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -943,7 +943,7 @@
         <v>23</v>
       </c>
       <c r="C49">
-        <v>194.40175438596739</v>
+        <v>210.53812500001419</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -954,7 +954,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <v>181.20483870965791</v>
+        <v>189.62408602150481</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -965,7 +965,7 @@
         <v>1</v>
       </c>
       <c r="C51">
-        <v>180.6145161290375</v>
+        <v>192.1391666666581</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -976,7 +976,7 @@
         <v>2</v>
       </c>
       <c r="C52">
-        <v>184.5145161290495</v>
+        <v>197.68959677420679</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -987,7 +987,7 @@
         <v>3</v>
       </c>
       <c r="C53">
-        <v>203.74032258060609</v>
+        <v>216.53123655911361</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -998,7 +998,7 @@
         <v>4</v>
       </c>
       <c r="C54">
-        <v>209.00806451614409</v>
+        <v>226.9500268817346</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1009,7 +1009,7 @@
         <v>5</v>
       </c>
       <c r="C55">
-        <v>212.04516129028951</v>
+        <v>229.69413978491411</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1020,7 +1020,7 @@
         <v>6</v>
       </c>
       <c r="C56">
-        <v>201.62903225810581</v>
+        <v>217.48572580648241</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1031,7 +1031,7 @@
         <v>7</v>
       </c>
       <c r="C57">
-        <v>184.33064516129781</v>
+        <v>198.9392741935533</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1042,7 +1042,7 @@
         <v>8</v>
       </c>
       <c r="C58">
-        <v>171.63225806451541</v>
+        <v>185.24400537635341</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1053,7 +1053,7 @@
         <v>9</v>
       </c>
       <c r="C59">
-        <v>161.45573770489969</v>
+        <v>174.7181571815475</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1064,7 +1064,7 @@
         <v>10</v>
       </c>
       <c r="C60">
-        <v>157.12786885247121</v>
+        <v>167.5883114446732</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1075,7 +1075,7 @@
         <v>11</v>
       </c>
       <c r="C61">
-        <v>151.08709677417329</v>
+        <v>161.57386709889019</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1086,7 +1086,7 @@
         <v>12</v>
       </c>
       <c r="C62">
-        <v>147.87903225807949</v>
+        <v>155.59471644121811</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1097,7 +1097,7 @@
         <v>13</v>
       </c>
       <c r="C63">
-        <v>147.06129032253631</v>
+        <v>153.86255376340799</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1108,7 +1108,7 @@
         <v>14</v>
       </c>
       <c r="C64">
-        <v>148.7274193548665</v>
+        <v>156.51045698927939</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1119,7 +1119,7 @@
         <v>15</v>
       </c>
       <c r="C65">
-        <v>157.42903225804719</v>
+        <v>165.83376344085119</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1130,7 +1130,7 @@
         <v>16</v>
       </c>
       <c r="C66">
-        <v>171.40322580647791</v>
+        <v>180.2697043010717</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1141,7 +1141,7 @@
         <v>17</v>
       </c>
       <c r="C67">
-        <v>192.43870967741111</v>
+        <v>203.48564516129201</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1152,7 +1152,7 @@
         <v>18</v>
       </c>
       <c r="C68">
-        <v>202.70322580646811</v>
+        <v>213.45376344086441</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1163,7 +1163,7 @@
         <v>19</v>
       </c>
       <c r="C69">
-        <v>200.31935483869921</v>
+        <v>209.05809325176941</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1174,7 +1174,7 @@
         <v>20</v>
       </c>
       <c r="C70">
-        <v>185.34354838710499</v>
+        <v>195.83865406005941</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -1185,7 +1185,7 @@
         <v>21</v>
       </c>
       <c r="C71">
-        <v>179.2516129032048</v>
+        <v>185.54255376342641</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -1196,7 +1196,7 @@
         <v>22</v>
       </c>
       <c r="C72">
-        <v>175.62580645164749</v>
+        <v>182.90629032260179</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -1207,7 +1207,7 @@
         <v>23</v>
       </c>
       <c r="C73">
-        <v>170.1306451612918</v>
+        <v>180.97550135501751</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1218,7 +1218,7 @@
         <v>0</v>
       </c>
       <c r="C74">
-        <v>135.18666666669299</v>
+        <v>150.12418103450329</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -1229,7 +1229,7 @@
         <v>1</v>
       </c>
       <c r="C75">
-        <v>138.20833333333329</v>
+        <v>154.23511111110369</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -1240,7 +1240,7 @@
         <v>2</v>
       </c>
       <c r="C76">
-        <v>149.06333333331861</v>
+        <v>168.12855555556021</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -1251,7 +1251,7 @@
         <v>3</v>
       </c>
       <c r="C77">
-        <v>163.17333333331629</v>
+        <v>183.21035931898609</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -1262,7 +1262,7 @@
         <v>4</v>
       </c>
       <c r="C78">
-        <v>166.14666666667131</v>
+        <v>186.6989499311361</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -1273,7 +1273,7 @@
         <v>5</v>
       </c>
       <c r="C79">
-        <v>154.4450000000225</v>
+        <v>173.63599630543229</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -1284,7 +1284,7 @@
         <v>6</v>
       </c>
       <c r="C80">
-        <v>144.67499999998839</v>
+        <v>162.06672222221289</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -1295,7 +1295,7 @@
         <v>7</v>
       </c>
       <c r="C81">
-        <v>135.46666666665891</v>
+        <v>152.95402777779569</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -1306,7 +1306,7 @@
         <v>8</v>
       </c>
       <c r="C82">
-        <v>128.60833333334111</v>
+        <v>144.94994444443441</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -1317,7 +1317,7 @@
         <v>9</v>
       </c>
       <c r="C83">
-        <v>124.9849999999938</v>
+        <v>140.3727499999863</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -1328,7 +1328,7 @@
         <v>10</v>
       </c>
       <c r="C84">
-        <v>121.7316666666341</v>
+        <v>136.0902222222231</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -1339,7 +1339,7 @@
         <v>11</v>
       </c>
       <c r="C85">
-        <v>116.70666666668841</v>
+        <v>130.35586111110749</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -1350,7 +1350,7 @@
         <v>12</v>
       </c>
       <c r="C86">
-        <v>115.87499999997669</v>
+        <v>128.61034126982361</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -1361,7 +1361,7 @@
         <v>13</v>
       </c>
       <c r="C87">
-        <v>115.8966666666868</v>
+        <v>128.53066141834131</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -1372,7 +1372,7 @@
         <v>14</v>
       </c>
       <c r="C88">
-        <v>117.07333333333951</v>
+        <v>131.0653862007195</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -1383,7 +1383,7 @@
         <v>15</v>
       </c>
       <c r="C89">
-        <v>121.5516666666682</v>
+        <v>137.27927777778049</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -1394,7 +1394,7 @@
         <v>16</v>
       </c>
       <c r="C90">
-        <v>136.1466666666519</v>
+        <v>151.21195788529491</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -1405,7 +1405,7 @@
         <v>17</v>
       </c>
       <c r="C91">
-        <v>150.63166666664961</v>
+        <v>167.39979211470441</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -1416,7 +1416,7 @@
         <v>18</v>
       </c>
       <c r="C92">
-        <v>158.2116666667047</v>
+        <v>174.18902777778371</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -1427,7 +1427,7 @@
         <v>19</v>
       </c>
       <c r="C93">
-        <v>151.48833333333411</v>
+        <v>165.79933333333369</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -1438,7 +1438,7 @@
         <v>20</v>
       </c>
       <c r="C94">
-        <v>139.70666666665349</v>
+        <v>152.0766388888878</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -1449,7 +1449,7 @@
         <v>21</v>
       </c>
       <c r="C95">
-        <v>132.82333333335509</v>
+        <v>145.48780555555709</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -1460,7 +1460,7 @@
         <v>22</v>
       </c>
       <c r="C96">
-        <v>131.09333333334649</v>
+        <v>144.90436111113911</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -1471,7 +1471,7 @@
         <v>23</v>
       </c>
       <c r="C97">
-        <v>132.30666666664959</v>
+        <v>147.52987452104671</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -1482,7 +1482,7 @@
         <v>0</v>
       </c>
       <c r="C98">
-        <v>75.253225806424581</v>
+        <v>82.70682795697283</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -1493,7 +1493,7 @@
         <v>1</v>
       </c>
       <c r="C99">
-        <v>76.867741935522176</v>
+        <v>83.968790322596647</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -1504,7 +1504,7 @@
         <v>2</v>
       </c>
       <c r="C100">
-        <v>82.946774193528853</v>
+        <v>90.323709677413831</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -1515,7 +1515,7 @@
         <v>3</v>
       </c>
       <c r="C101">
-        <v>93.777419354826691</v>
+        <v>100.3655376343917</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -1526,7 +1526,7 @@
         <v>4</v>
       </c>
       <c r="C102">
-        <v>90.361290322612945</v>
+        <v>97.901236559145133</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -1537,7 +1537,7 @@
         <v>5</v>
       </c>
       <c r="C103">
-        <v>81.170967741955764</v>
+        <v>88.838844086051054</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -1548,7 +1548,7 @@
         <v>6</v>
       </c>
       <c r="C104">
-        <v>79.019354838678879</v>
+        <v>85.648790322551164</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -1559,7 +1559,7 @@
         <v>7</v>
       </c>
       <c r="C105">
-        <v>79.532258064538667</v>
+        <v>85.127365591410069</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -1570,7 +1570,7 @@
         <v>8</v>
       </c>
       <c r="C106">
-        <v>77.838709677415594</v>
+        <v>82.930913978505075</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -1581,7 +1581,7 @@
         <v>9</v>
       </c>
       <c r="C107">
-        <v>77.822580645135005</v>
+        <v>82.792607526869446</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -1592,7 +1592,7 @@
         <v>10</v>
       </c>
       <c r="C108">
-        <v>76.945161290305307</v>
+        <v>81.846075268790898</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -1603,7 +1603,7 @@
         <v>11</v>
       </c>
       <c r="C109">
-        <v>74.611290322627966</v>
+        <v>79.862956989281471</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -1614,7 +1614,7 @@
         <v>12</v>
       </c>
       <c r="C110">
-        <v>72.206451612881452</v>
+        <v>77.784139784935476</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -1625,7 +1625,7 @@
         <v>13</v>
       </c>
       <c r="C111">
-        <v>70.732258064525894</v>
+        <v>76.688145161290919</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -1636,7 +1636,7 @@
         <v>14</v>
       </c>
       <c r="C112">
-        <v>72.27096774197004</v>
+        <v>77.967258064541966</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -1647,7 +1647,7 @@
         <v>15</v>
       </c>
       <c r="C113">
-        <v>75.883870967682597</v>
+        <v>82.208172042977111</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -1658,7 +1658,7 @@
         <v>16</v>
       </c>
       <c r="C114">
-        <v>82.851612903237822</v>
+        <v>90.338091397857966</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -1669,7 +1669,7 @@
         <v>17</v>
       </c>
       <c r="C115">
-        <v>92.749999999996248</v>
+        <v>100.0174462365507</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -1680,7 +1680,7 @@
         <v>18</v>
       </c>
       <c r="C116">
-        <v>96.253225806443353</v>
+        <v>104.7540860214973</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -1691,7 +1691,7 @@
         <v>19</v>
       </c>
       <c r="C117">
-        <v>89.896774193598702</v>
+        <v>99.101559139818193</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -1702,7 +1702,7 @@
         <v>20</v>
       </c>
       <c r="C118">
-        <v>81.05645161287319</v>
+        <v>89.588145161286036</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -1713,7 +1713,7 @@
         <v>21</v>
       </c>
       <c r="C119">
-        <v>72.441935483850685</v>
+        <v>80.888629032231322</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -1724,7 +1724,7 @@
         <v>22</v>
       </c>
       <c r="C120">
-        <v>72.716129032282851</v>
+        <v>80.316129032285858</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -1735,7 +1735,7 @@
         <v>23</v>
       </c>
       <c r="C121">
-        <v>73.109677419336819</v>
+        <v>80.668010752678157</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -1746,7 +1746,7 @@
         <v>0</v>
       </c>
       <c r="C122">
-        <v>39.82666666670314</v>
+        <v>38.287316384224091</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -1757,7 +1757,7 @@
         <v>1</v>
       </c>
       <c r="C123">
-        <v>40.456666666661228</v>
+        <v>38.890225988680541</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -1768,7 +1768,7 @@
         <v>2</v>
       </c>
       <c r="C124">
-        <v>41.98666666666977</v>
+        <v>40.780903954805723</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -1779,7 +1779,7 @@
         <v>3</v>
       </c>
       <c r="C125">
-        <v>49.951666666672097</v>
+        <v>48.51016949154377</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -1790,7 +1790,7 @@
         <v>4</v>
       </c>
       <c r="C126">
-        <v>51.639999999979047</v>
+        <v>50.712485875671938</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -1801,7 +1801,7 @@
         <v>5</v>
       </c>
       <c r="C127">
-        <v>50.65500000002406</v>
+        <v>49.572203389845463</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -1812,7 +1812,7 @@
         <v>6</v>
       </c>
       <c r="C128">
-        <v>49.803333333317028</v>
+        <v>48.784802259886213</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -1823,7 +1823,7 @@
         <v>7</v>
       </c>
       <c r="C129">
-        <v>51.069999999972062</v>
+        <v>50.294901960769067</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -1834,7 +1834,7 @@
         <v>8</v>
       </c>
       <c r="C130">
-        <v>50.53999999999845</v>
+        <v>49.502661064417808</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -1845,7 +1845,7 @@
         <v>9</v>
       </c>
       <c r="C131">
-        <v>51.466666666666669</v>
+        <v>50.357002801128793</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -1856,7 +1856,7 @@
         <v>10</v>
       </c>
       <c r="C132">
-        <v>51.803333333375242</v>
+        <v>50.463473389374222</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -1867,7 +1867,7 @@
         <v>11</v>
       </c>
       <c r="C133">
-        <v>50.064999999979037</v>
+        <v>48.732352941163953</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -1878,7 +1878,7 @@
         <v>12</v>
       </c>
       <c r="C134">
-        <v>48.995000000010869</v>
+        <v>47.672231638449901</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -1889,7 +1889,7 @@
         <v>13</v>
       </c>
       <c r="C135">
-        <v>47.924999999988358</v>
+        <v>47.014632768327203</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -1900,7 +1900,7 @@
         <v>14</v>
       </c>
       <c r="C136">
-        <v>47.745000000022507</v>
+        <v>46.774689265547551</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -1911,7 +1911,7 @@
         <v>15</v>
       </c>
       <c r="C137">
-        <v>48.88833333333411</v>
+        <v>48.796441589214773</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -1922,7 +1922,7 @@
         <v>16</v>
       </c>
       <c r="C138">
-        <v>53.866666666662788</v>
+        <v>53.827004738471679</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -1933,7 +1933,7 @@
         <v>17</v>
       </c>
       <c r="C139">
-        <v>60.053333333313162</v>
+        <v>60.578983050848997</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -1944,7 +1944,7 @@
         <v>18</v>
       </c>
       <c r="C140">
-        <v>61.253333333324797</v>
+        <v>61.885338983043702</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -1955,7 +1955,7 @@
         <v>19</v>
       </c>
       <c r="C141">
-        <v>54.754999999993018</v>
+        <v>54.769073264066613</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -1966,7 +1966,7 @@
         <v>20</v>
       </c>
       <c r="C142">
-        <v>48.173333333362827</v>
+        <v>47.737367413894638</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -1977,7 +1977,7 @@
         <v>21</v>
       </c>
       <c r="C143">
-        <v>41.336666666658132</v>
+        <v>39.563615819204493</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -1988,7 +1988,7 @@
         <v>22</v>
       </c>
       <c r="C144">
-        <v>41.508333333321687</v>
+        <v>39.120508474579978</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -1999,7 +1999,7 @@
         <v>23</v>
       </c>
       <c r="C145">
-        <v>41.113333333334111</v>
+        <v>38.370112994341447</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -2010,7 +2010,7 @@
         <v>0</v>
       </c>
       <c r="C146">
-        <v>31.17580645163018</v>
+        <v>34.286396396391488</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -2021,7 +2021,7 @@
         <v>1</v>
       </c>
       <c r="C147">
-        <v>30.762903225750868</v>
+        <v>34.416666666632047</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -2032,7 +2032,7 @@
         <v>2</v>
       </c>
       <c r="C148">
-        <v>32.50645161293928</v>
+        <v>35.399026548710403</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -2043,7 +2043,7 @@
         <v>3</v>
       </c>
       <c r="C149">
-        <v>38.069354838710431</v>
+        <v>42.178141592922458</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -2054,7 +2054,7 @@
         <v>4</v>
       </c>
       <c r="C150">
-        <v>39.100000000006759</v>
+        <v>43.153008849569183</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -2065,7 +2065,7 @@
         <v>5</v>
       </c>
       <c r="C151">
-        <v>37.598387096741902</v>
+        <v>41.569616519138258</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -2076,7 +2076,7 @@
         <v>6</v>
       </c>
       <c r="C152">
-        <v>37.896774193538633</v>
+        <v>41.958584070788802</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -2087,7 +2087,7 @@
         <v>7</v>
       </c>
       <c r="C153">
-        <v>38.537096774239373</v>
+        <v>46.530117994137271</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -2098,7 +2098,7 @@
         <v>8</v>
       </c>
       <c r="C154">
-        <v>37.627419354822187</v>
+        <v>43.816578171071718</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -2109,7 +2109,7 @@
         <v>9</v>
       </c>
       <c r="C155">
-        <v>38.041935483876223</v>
+        <v>44.29471976403147</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -2120,7 +2120,7 @@
         <v>10</v>
       </c>
       <c r="C156">
-        <v>37.043548387069727</v>
+        <v>43.165604719736578</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -2131,7 +2131,7 @@
         <v>11</v>
       </c>
       <c r="C157">
-        <v>35.579032258081789</v>
+        <v>41.652172619049708</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -2142,7 +2142,7 @@
         <v>12</v>
       </c>
       <c r="C158">
-        <v>35.012903225773407</v>
+        <v>40.958214285699277</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -2153,7 +2153,7 @@
         <v>13</v>
       </c>
       <c r="C159">
-        <v>34.51290322585227</v>
+        <v>40.851428571458591</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -2164,7 +2164,7 @@
         <v>14</v>
       </c>
       <c r="C160">
-        <v>34.159677419345833</v>
+        <v>40.410565476191032</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -2175,7 +2175,7 @@
         <v>15</v>
       </c>
       <c r="C161">
-        <v>35.961290322574627</v>
+        <v>41.674985250734217</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -2186,7 +2186,7 @@
         <v>16</v>
       </c>
       <c r="C162">
-        <v>39.88387096776146</v>
+        <v>45.203157894751428</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -2197,7 +2197,7 @@
         <v>17</v>
       </c>
       <c r="C163">
-        <v>45.393548387095272</v>
+        <v>49.826405797088917</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -2208,7 +2208,7 @@
         <v>18</v>
       </c>
       <c r="C164">
-        <v>46.795161290312073</v>
+        <v>50.949739130435553</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -2219,7 +2219,7 @@
         <v>19</v>
       </c>
       <c r="C165">
-        <v>43.559677419354088</v>
+        <v>47.382138535991032</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -2230,7 +2230,7 @@
         <v>20</v>
       </c>
       <c r="C166">
-        <v>37.256451612916742</v>
+        <v>41.428963482858968</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -2241,7 +2241,7 @@
         <v>21</v>
       </c>
       <c r="C167">
-        <v>30.211290322582151</v>
+        <v>34.031160714291858</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -2252,7 +2252,7 @@
         <v>22</v>
       </c>
       <c r="C168">
-        <v>30.453225806404291</v>
+        <v>34.512142857114668</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -2263,7 +2263,7 @@
         <v>23</v>
       </c>
       <c r="C169">
-        <v>30.93064516131961</v>
+        <v>34.598727272755717</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -2274,7 +2274,7 @@
         <v>0</v>
       </c>
       <c r="C170">
-        <v>29.091935483900262</v>
+        <v>35.002672955974766</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -2285,7 +2285,7 @@
         <v>1</v>
       </c>
       <c r="C171">
-        <v>29.687096774183789</v>
+        <v>35.643679245276253</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -2296,7 +2296,7 @@
         <v>2</v>
       </c>
       <c r="C172">
-        <v>31.485483870976751</v>
+        <v>36.695919003135252</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -2307,7 +2307,7 @@
         <v>3</v>
       </c>
       <c r="C173">
-        <v>36.448387096759923</v>
+        <v>42.432716049373589</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -2318,7 +2318,7 @@
         <v>4</v>
       </c>
       <c r="C174">
-        <v>38.685483870956467</v>
+        <v>45.356352201252207</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -2329,7 +2329,7 @@
         <v>5</v>
       </c>
       <c r="C175">
-        <v>38.425806451633932</v>
+        <v>44.328285714298751</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -2340,7 +2340,7 @@
         <v>6</v>
       </c>
       <c r="C176">
-        <v>38.208064516108763</v>
+        <v>44.869182389937912</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -2351,7 +2351,7 @@
         <v>7</v>
       </c>
       <c r="C177">
-        <v>36.980645161294831</v>
+        <v>44.855943396216347</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -2362,7 +2362,7 @@
         <v>8</v>
       </c>
       <c r="C178">
-        <v>36.142622950849443</v>
+        <v>44.428480725642302</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -2373,7 +2373,7 @@
         <v>9</v>
       </c>
       <c r="C179">
-        <v>35.729032258037478</v>
+        <v>44.251632756550293</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -2384,7 +2384,7 @@
         <v>10</v>
       </c>
       <c r="C180">
-        <v>35.42580645158511</v>
+        <v>43.692551865385447</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -2395,7 +2395,7 @@
         <v>11</v>
       </c>
       <c r="C181">
-        <v>40.408064516148563</v>
+        <v>45.200398467434567</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -2406,7 +2406,7 @@
         <v>12</v>
       </c>
       <c r="C182">
-        <v>34.762903225803448</v>
+        <v>42.089496855343967</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -2417,7 +2417,7 @@
         <v>13</v>
       </c>
       <c r="C183">
-        <v>33.25000000001878</v>
+        <v>41.744528301894867</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -2428,7 +2428,7 @@
         <v>14</v>
       </c>
       <c r="C184">
-        <v>33.219354838666113</v>
+        <v>41.022672955949467</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
@@ -2439,7 +2439,7 @@
         <v>15</v>
       </c>
       <c r="C185">
-        <v>34.545161290364639</v>
+        <v>41.70910838976063</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
@@ -2450,7 +2450,7 @@
         <v>16</v>
       </c>
       <c r="C186">
-        <v>36.764516129019491</v>
+        <v>44.618669646646588</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
@@ -2461,7 +2461,7 @@
         <v>17</v>
       </c>
       <c r="C187">
-        <v>39.833870967752453</v>
+        <v>49.098842541109427</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -2472,7 +2472,7 @@
         <v>18</v>
       </c>
       <c r="C188">
-        <v>41.149999999993241</v>
+        <v>51.074898000192938</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
@@ -2483,7 +2483,7 @@
         <v>19</v>
       </c>
       <c r="C189">
-        <v>38.359677419366847</v>
+        <v>47.108722741435997</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
@@ -2494,7 +2494,7 @@
         <v>20</v>
       </c>
       <c r="C190">
-        <v>33.443548387070493</v>
+        <v>41.333553459117503</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
@@ -2505,7 +2505,7 @@
         <v>21</v>
       </c>
       <c r="C191">
-        <v>27.795161290323328</v>
+        <v>33.827999999981728</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
@@ -2516,7 +2516,7 @@
         <v>22</v>
       </c>
       <c r="C192">
-        <v>28.185483870963981</v>
+        <v>33.41261682242795</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
@@ -2527,7 +2527,7 @@
         <v>23</v>
       </c>
       <c r="C193">
-        <v>29.840322580654171</v>
+        <v>34.311775700949681</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
@@ -2538,7 +2538,7 @@
         <v>0</v>
       </c>
       <c r="C194">
-        <v>48.476666666656577</v>
+        <v>53.751960784310327</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -2549,7 +2549,7 @@
         <v>1</v>
       </c>
       <c r="C195">
-        <v>49.890000000045013</v>
+        <v>55.277338935608171</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -2560,7 +2560,7 @@
         <v>2</v>
       </c>
       <c r="C196">
-        <v>53.993333333299958</v>
+        <v>59.827591036403348</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -2571,7 +2571,7 @@
         <v>3</v>
       </c>
       <c r="C197">
-        <v>63.651666666672099</v>
+        <v>69.440252100834584</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -2582,7 +2582,7 @@
         <v>4</v>
       </c>
       <c r="C198">
-        <v>66.305000000016292</v>
+        <v>72.268431372551191</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -2593,7 +2593,7 @@
         <v>5</v>
       </c>
       <c r="C199">
-        <v>65.038333333330229</v>
+        <v>72.350444444438708</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
@@ -2604,7 +2604,7 @@
         <v>6</v>
       </c>
       <c r="C200">
-        <v>63.956666666676753</v>
+        <v>70.717622222242056</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
@@ -2615,7 +2615,7 @@
         <v>7</v>
       </c>
       <c r="C201">
-        <v>65.113333333353509</v>
+        <v>70.785877777774786</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
@@ -2626,7 +2626,7 @@
         <v>8</v>
       </c>
       <c r="C202">
-        <v>64.188333333330235</v>
+        <v>68.681055555569273</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
@@ -2637,7 +2637,7 @@
         <v>9</v>
       </c>
       <c r="C203">
-        <v>62.829999999977503</v>
+        <v>67.333999999989956</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
@@ -2648,7 +2648,7 @@
         <v>10</v>
       </c>
       <c r="C204">
-        <v>62.338333333349631</v>
+        <v>66.723138888894269</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
@@ -2659,7 +2659,7 @@
         <v>11</v>
       </c>
       <c r="C205">
-        <v>61.031666666665117</v>
+        <v>64.898527777775115</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
@@ -2670,7 +2670,7 @@
         <v>12</v>
       </c>
       <c r="C206">
-        <v>58.4266666666527</v>
+        <v>62.966333333324293</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
@@ -2681,7 +2681,7 @@
         <v>13</v>
       </c>
       <c r="C207">
-        <v>57.153333333355839</v>
+        <v>62.585166666670311</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
@@ -2692,7 +2692,7 @@
         <v>14</v>
       </c>
       <c r="C208">
-        <v>58.586666666642607</v>
+        <v>64.280999999992005</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
@@ -2703,7 +2703,7 @@
         <v>15</v>
       </c>
       <c r="C209">
-        <v>60.545000000010873</v>
+        <v>67.26058333332476</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
@@ -2714,7 +2714,7 @@
         <v>16</v>
       </c>
       <c r="C210">
-        <v>68.708333333306172</v>
+        <v>76.165194444438868</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
@@ -2725,7 +2725,7 @@
         <v>17</v>
       </c>
       <c r="C211">
-        <v>75.843333333346521</v>
+        <v>86.226653225819845</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
@@ -2736,7 +2736,7 @@
         <v>18</v>
       </c>
       <c r="C212">
-        <v>74.604999999989133</v>
+        <v>84.448235663075081</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
@@ -2747,7 +2747,7 @@
         <v>19</v>
       </c>
       <c r="C213">
-        <v>65.131666666661232</v>
+        <v>73.987249999998795</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
@@ -2758,7 +2758,7 @@
         <v>20</v>
       </c>
       <c r="C214">
-        <v>56.206666666672866</v>
+        <v>63.735027777789703</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
@@ -2769,7 +2769,7 @@
         <v>21</v>
       </c>
       <c r="C215">
-        <v>48.973333333324021</v>
+        <v>57.02058823527905</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
@@ -2780,7 +2780,7 @@
         <v>22</v>
       </c>
       <c r="C216">
-        <v>48.821666666671327</v>
+        <v>56.835070028007927</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
@@ -2791,7 +2791,7 @@
         <v>23</v>
       </c>
       <c r="C217">
-        <v>49.313333333326348</v>
+        <v>56.519887955179399</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
@@ -2802,7 +2802,7 @@
         <v>0</v>
       </c>
       <c r="C218">
-        <v>109.97580645165419</v>
+        <v>117.9368010752904</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
@@ -2813,7 +2813,7 @@
         <v>1</v>
       </c>
       <c r="C219">
-        <v>112.52419354837581</v>
+        <v>120.5366397849369</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
@@ -2824,7 +2824,7 @@
         <v>2</v>
       </c>
       <c r="C220">
-        <v>121.9951612903218</v>
+        <v>130.57631720430331</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
@@ -2835,7 +2835,7 @@
         <v>3</v>
       </c>
       <c r="C221">
-        <v>137.57419354837731</v>
+        <v>145.85182795700359</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
@@ -2846,7 +2846,7 @@
         <v>4</v>
       </c>
       <c r="C222">
-        <v>142.06774193549811</v>
+        <v>149.33965053762901</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
@@ -2857,7 +2857,7 @@
         <v>5</v>
       </c>
       <c r="C223">
-        <v>139.29354838708849</v>
+        <v>147.27908602150649</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
@@ -2868,7 +2868,7 @@
         <v>6</v>
       </c>
       <c r="C224">
-        <v>137.32096774193019</v>
+        <v>143.72010752687979</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
@@ -2879,7 +2879,7 @@
         <v>7</v>
       </c>
       <c r="C225">
-        <v>129.30322580646359</v>
+        <v>131.83190860215859</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
@@ -2890,7 +2890,7 @@
         <v>8</v>
       </c>
       <c r="C226">
-        <v>122.0887096774043</v>
+        <v>122.9297432332035</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
@@ -2901,7 +2901,7 @@
         <v>9</v>
       </c>
       <c r="C227">
-        <v>116.7000000000323</v>
+        <v>116.370699014449</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
@@ -2912,7 +2912,7 @@
         <v>10</v>
       </c>
       <c r="C228">
-        <v>111.4387096773998</v>
+        <v>111.4128910856774</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
@@ -2923,7 +2923,7 @@
         <v>11</v>
       </c>
       <c r="C229">
-        <v>107.348387096802</v>
+        <v>106.5594768403643</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
@@ -2934,7 +2934,7 @@
         <v>12</v>
       </c>
       <c r="C230">
-        <v>108.1677419354636</v>
+        <v>105.7545822994293</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
@@ -2945,7 +2945,7 @@
         <v>13</v>
       </c>
       <c r="C231">
-        <v>109.2483870967727</v>
+        <v>107.72157181571311</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
@@ -2956,7 +2956,7 @@
         <v>14</v>
       </c>
       <c r="C232">
-        <v>112.72903225807499</v>
+        <v>111.8085365853683</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
@@ -2967,7 +2967,7 @@
         <v>15</v>
       </c>
       <c r="C233">
-        <v>121.0951612903098</v>
+        <v>124.3575806451469</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
@@ -2978,7 +2978,7 @@
         <v>16</v>
       </c>
       <c r="C234">
-        <v>135.4322580645094</v>
+        <v>140.4509677419471</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
@@ -2989,7 +2989,7 @@
         <v>17</v>
       </c>
       <c r="C235">
-        <v>142.81774193549811</v>
+        <v>150.38469377565079</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
@@ -3000,7 +3000,7 @@
         <v>18</v>
       </c>
       <c r="C236">
-        <v>138.5112903225874</v>
+        <v>146.31970138563361</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
@@ -3011,7 +3011,7 @@
         <v>19</v>
       </c>
       <c r="C237">
-        <v>129.6290322580457</v>
+        <v>138.00245794310561</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
@@ -3022,7 +3022,7 @@
         <v>20</v>
       </c>
       <c r="C238">
-        <v>117.83387096774869</v>
+        <v>125.12010926119009</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
@@ -3033,7 +3033,7 @@
         <v>21</v>
       </c>
       <c r="C239">
-        <v>108.14193548387919</v>
+        <v>116.8152956989492</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
@@ -3044,7 +3044,7 @@
         <v>22</v>
       </c>
       <c r="C240">
-        <v>106.706451612904</v>
+        <v>115.68099462364199</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
@@ -3055,7 +3055,7 @@
         <v>23</v>
       </c>
       <c r="C241">
-        <v>109.17580645157381</v>
+        <v>117.66163978491809</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
@@ -3066,7 +3066,7 @@
         <v>0</v>
       </c>
       <c r="C242">
-        <v>178.7033333333481</v>
+        <v>175.92279211470739</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
@@ -3077,7 +3077,7 @@
         <v>1</v>
       </c>
       <c r="C243">
-        <v>181.82333333333571</v>
+        <v>178.29723566307709</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
@@ -3088,7 +3088,7 @@
         <v>2</v>
       </c>
       <c r="C244">
-        <v>186.00833333331781</v>
+        <v>181.08730555553919</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
@@ -3099,7 +3099,7 @@
         <v>3</v>
       </c>
       <c r="C245">
-        <v>209.7316666666496</v>
+        <v>201.5233333333376</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
@@ -3110,7 +3110,7 @@
         <v>4</v>
       </c>
       <c r="C246">
-        <v>219.36166666670471</v>
+        <v>210.66769444445569</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
@@ -3121,7 +3121,7 @@
         <v>5</v>
       </c>
       <c r="C247">
-        <v>223.56666666665501</v>
+        <v>214.33924999999391</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
@@ -3132,7 +3132,7 @@
         <v>6</v>
       </c>
       <c r="C248">
-        <v>224.0916666666279</v>
+        <v>215.84023467431149</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
@@ -3143,7 +3143,7 @@
         <v>7</v>
       </c>
       <c r="C249">
-        <v>219.19666666667521</v>
+        <v>211.38323754790471</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
@@ -3154,7 +3154,7 @@
         <v>8</v>
       </c>
       <c r="C250">
-        <v>205.79833333333559</v>
+        <v>199.42775000000739</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
@@ -3165,7 +3165,7 @@
         <v>9</v>
       </c>
       <c r="C251">
-        <v>197.433333333376</v>
+        <v>191.1512729885163</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
@@ -3176,7 +3176,7 @@
         <v>10</v>
       </c>
       <c r="C252">
-        <v>191.93833333331469</v>
+        <v>186.24525478925591</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
@@ -3187,7 +3187,7 @@
         <v>11</v>
       </c>
       <c r="C253">
-        <v>185.04166666670159</v>
+        <v>180.5506851852154</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
@@ -3198,7 +3198,7 @@
         <v>12</v>
       </c>
       <c r="C254">
-        <v>183.66833333330379</v>
+        <v>179.4938981481294</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
@@ -3209,7 +3209,7 @@
         <v>13</v>
       </c>
       <c r="C255">
-        <v>185.47833333333261</v>
+        <v>180.60016666666971</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
@@ -3220,7 +3220,7 @@
         <v>14</v>
       </c>
       <c r="C256">
-        <v>190.9983333333046</v>
+        <v>186.11391666664471</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
@@ -3231,7 +3231,7 @@
         <v>15</v>
       </c>
       <c r="C257">
-        <v>202.92166666666739</v>
+        <v>197.13427777776769</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
@@ -3242,7 +3242,7 @@
         <v>16</v>
       </c>
       <c r="C258">
-        <v>211.63333333334501</v>
+        <v>205.5893333333506</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
@@ -3253,7 +3253,7 @@
         <v>17</v>
       </c>
       <c r="C259">
-        <v>214.0733333333512</v>
+        <v>210.27463888890239</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
@@ -3264,7 +3264,7 @@
         <v>18</v>
       </c>
       <c r="C260">
-        <v>217.7566666667</v>
+        <v>214.92969444444651</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
@@ -3275,7 +3275,7 @@
         <v>19</v>
       </c>
       <c r="C261">
-        <v>211.97833333330539</v>
+        <v>210.64105555555139</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
@@ -3286,7 +3286,7 @@
         <v>20</v>
       </c>
       <c r="C262">
-        <v>194.60999999996281</v>
+        <v>193.2999444444159</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
@@ -3297,7 +3297,7 @@
         <v>21</v>
       </c>
       <c r="C263">
-        <v>186.7600000000248</v>
+        <v>184.47705555557431</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
@@ -3308,7 +3308,7 @@
         <v>22</v>
       </c>
       <c r="C264">
-        <v>181.39833333332791</v>
+        <v>179.5510555555646</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
@@ -3319,7 +3319,7 @@
         <v>23</v>
       </c>
       <c r="C265">
-        <v>178.6316666666612</v>
+        <v>175.08044444443951</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
@@ -3330,7 +3330,7 @@
         <v>0</v>
       </c>
       <c r="C266">
-        <v>212.2838709677284</v>
+        <v>216.61991935481521</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
@@ -3341,7 +3341,7 @@
         <v>1</v>
       </c>
       <c r="C267">
-        <v>215.1032258064651</v>
+        <v>218.62024193547941</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
@@ -3352,7 +3352,7 @@
         <v>2</v>
       </c>
       <c r="C268">
-        <v>219.70483870966919</v>
+        <v>222.23088709678271</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
@@ -3363,7 +3363,7 @@
         <v>3</v>
       </c>
       <c r="C269">
-        <v>243.9096774193421</v>
+        <v>243.95008064516361</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
@@ -3374,7 +3374,7 @@
         <v>4</v>
       </c>
       <c r="C270">
-        <v>251.0274193548567</v>
+        <v>250.95080645161781</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
@@ -3385,7 +3385,7 @@
         <v>5</v>
       </c>
       <c r="C271">
-        <v>252.42741935483119</v>
+        <v>252.28852150537969</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
@@ -3396,7 +3396,7 @@
         <v>6</v>
       </c>
       <c r="C272">
-        <v>254.61612903225361</v>
+        <v>255.40529359221239</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
@@ -3407,7 +3407,7 @@
         <v>7</v>
       </c>
       <c r="C273">
-        <v>260.18387096774052</v>
+        <v>260.90599759750728</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
@@ -3418,7 +3418,7 @@
         <v>8</v>
       </c>
       <c r="C274">
-        <v>253.87903225804951</v>
+        <v>253.12293901554341</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
@@ -3429,7 +3429,7 @@
         <v>9</v>
       </c>
       <c r="C275">
-        <v>240.52419354838341</v>
+        <v>240.20804655959361</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
@@ -3440,7 +3440,7 @@
         <v>10</v>
       </c>
       <c r="C276">
-        <v>233.1338709677502</v>
+        <v>233.54963183728981</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
@@ -3451,7 +3451,7 @@
         <v>11</v>
       </c>
       <c r="C277">
-        <v>227.6822580645244</v>
+        <v>227.7708064516041</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
@@ -3462,7 +3462,7 @@
         <v>12</v>
       </c>
       <c r="C278">
-        <v>223.95483870969551</v>
+        <v>225.0039516129182</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
@@ -3473,7 +3473,7 @@
         <v>13</v>
       </c>
       <c r="C279">
-        <v>224.55322580646359</v>
+        <v>226.58261424733041</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
@@ -3484,7 +3484,7 @@
         <v>14</v>
       </c>
       <c r="C280">
-        <v>230.03064516129629</v>
+        <v>232.70633736557531</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
@@ -3495,7 +3495,7 @@
         <v>15</v>
       </c>
       <c r="C281">
-        <v>239.40967741933079</v>
+        <v>241.16263440859339</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
@@ -3506,7 +3506,7 @@
         <v>16</v>
       </c>
       <c r="C282">
-        <v>241.83870967737431</v>
+        <v>243.91481182795019</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
@@ -3517,7 +3517,7 @@
         <v>17</v>
       </c>
       <c r="C283">
-        <v>243.71451612906679</v>
+        <v>247.07010752688569</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
@@ -3528,7 +3528,7 @@
         <v>18</v>
       </c>
       <c r="C284">
-        <v>247.97096774188589</v>
+        <v>251.93698924731069</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
@@ -3539,7 +3539,7 @@
         <v>19</v>
       </c>
       <c r="C285">
-        <v>243.60806451619209</v>
+        <v>248.5978494623578</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
@@ -3550,7 +3550,7 @@
         <v>20</v>
       </c>
       <c r="C286">
-        <v>228.97258064516211</v>
+        <v>234.1700806451864</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
@@ -3561,7 +3561,7 @@
         <v>21</v>
       </c>
       <c r="C287">
-        <v>221.38709677415969</v>
+        <v>224.3923924731038</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
@@ -3572,7 +3572,7 @@
         <v>22</v>
       </c>
       <c r="C288">
-        <v>215.2564516129205</v>
+        <v>218.8363440860262</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
@@ -3583,7 +3583,7 @@
         <v>23</v>
       </c>
       <c r="C289">
-        <v>209.8032258064824</v>
+        <v>212.68435483872361</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data z roku 23-24
</commit_message>
<xml_diff>
--- a/prumerna_dodavka_tepla.xlsx
+++ b/prumerna_dodavka_tepla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cezdata-my.sharepoint.com/personal/michal_pekarek01_cez_cz/Documents/Plocha/práce/#30 Prediktivní model EPRU/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_2B8B061F6721173CF2FE31D2F8F2D3C2C4DC5C93" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5EF6A76-7934-46AF-8173-829CBA01766F}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_C996061F02D9D301BEFE31D2F8F2D3C244D82BC1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CE57615-34D8-4C6A-9AD3-7F1679EB8DDB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -401,8 +401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
-      <selection activeCell="C276" sqref="C276"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,7 +426,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>222.99319783198251</v>
+        <v>224.3324731182675</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -437,7 +437,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>224.74543010752731</v>
+        <v>226.40967741936839</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -448,7 +448,7 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>226.91602150534561</v>
+        <v>229.04516129026331</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -459,7 +459,7 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>248.31972899733611</v>
+        <v>249.35322580651771</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -470,7 +470,7 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>257.20956639565361</v>
+        <v>253.21451612902169</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -481,7 +481,7 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>261.2523848238298</v>
+        <v>256.64999999996701</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -492,7 +492,7 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>263.16463414635137</v>
+        <v>259.03870967744041</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -503,7 +503,7 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>268.07755376347632</v>
+        <v>261.20508474580771</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -514,7 +514,7 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>258.90567204298861</v>
+        <v>247.8172413793047</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -525,7 +525,7 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>247.42571815717289</v>
+        <v>237.9274193548124</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -536,7 +536,7 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>240.19826558265339</v>
+        <v>229.69193548386571</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -547,7 +547,7 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>233.4906048386857</v>
+        <v>224.43606557372999</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -558,7 +558,7 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>228.65625000002021</v>
+        <v>220.0322580645537</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -569,7 +569,7 @@
         <v>13</v>
       </c>
       <c r="C15">
-        <v>229.67361617577899</v>
+        <v>222.16393442623709</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -580,7 +580,7 @@
         <v>14</v>
       </c>
       <c r="C16">
-        <v>234.97216339411389</v>
+        <v>227.7999999999752</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -591,7 +591,7 @@
         <v>15</v>
       </c>
       <c r="C17">
-        <v>245.59354838710269</v>
+        <v>239.64677419358739</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -602,7 +602,7 @@
         <v>16</v>
       </c>
       <c r="C18">
-        <v>256.01865591397723</v>
+        <v>252.23387096771941</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -613,7 +613,7 @@
         <v>17</v>
       </c>
       <c r="C19">
-        <v>261.50862903225828</v>
+        <v>259.03870967743279</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -624,7 +624,7 @@
         <v>18</v>
       </c>
       <c r="C20">
-        <v>265.24615591396503</v>
+        <v>264.08196721309952</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -635,7 +635,7 @@
         <v>19</v>
       </c>
       <c r="C21">
-        <v>262.19021505376338</v>
+        <v>262.09016393442238</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -646,7 +646,7 @@
         <v>20</v>
       </c>
       <c r="C22">
-        <v>246.32831978319879</v>
+        <v>244.30000000000899</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -657,7 +657,7 @@
         <v>21</v>
       </c>
       <c r="C23">
-        <v>233.14336043363201</v>
+        <v>236.51967213119261</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -668,7 +668,7 @@
         <v>22</v>
       </c>
       <c r="C24">
-        <v>227.74572580642351</v>
+        <v>228.95737704915589</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -679,7 +679,7 @@
         <v>23</v>
       </c>
       <c r="C25">
-        <v>220.91263440860789</v>
+        <v>223.13114754099499</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -690,7 +690,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <v>213.65502976189501</v>
+        <v>200.43035714285881</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -701,7 +701,7 @@
         <v>1</v>
       </c>
       <c r="C27">
-        <v>217.5491369047694</v>
+        <v>203.20178571429491</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -712,7 +712,7 @@
         <v>2</v>
       </c>
       <c r="C28">
-        <v>221.63309523809119</v>
+        <v>205.8339285714236</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -723,7 +723,7 @@
         <v>3</v>
       </c>
       <c r="C29">
-        <v>240.3453571428436</v>
+        <v>224.5618181817911</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -734,7 +734,7 @@
         <v>4</v>
       </c>
       <c r="C30">
-        <v>248.64002949852579</v>
+        <v>227.4947368421208</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -745,7 +745,7 @@
         <v>5</v>
       </c>
       <c r="C31">
-        <v>253.02179941005201</v>
+        <v>229.0298245614068</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -756,7 +756,7 @@
         <v>6</v>
       </c>
       <c r="C32">
-        <v>255.0911209439175</v>
+        <v>229.3017543859396</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -767,7 +767,7 @@
         <v>7</v>
       </c>
       <c r="C33">
-        <v>249.20262536874799</v>
+        <v>224.9163636363831</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -778,7 +778,7 @@
         <v>8</v>
       </c>
       <c r="C34">
-        <v>233.2724188790441</v>
+        <v>211.08888888888109</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -789,7 +789,7 @@
         <v>9</v>
       </c>
       <c r="C35">
-        <v>219.57252423096119</v>
+        <v>197.8339285714776</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -800,7 +800,7 @@
         <v>10</v>
       </c>
       <c r="C36">
-        <v>211.19485040033129</v>
+        <v>190.70178571428659</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -811,7 +811,7 @@
         <v>11</v>
       </c>
       <c r="C37">
-        <v>205.54772861356551</v>
+        <v>186.68421052629131</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -822,7 +822,7 @@
         <v>12</v>
       </c>
       <c r="C38">
-        <v>198.99179941002981</v>
+        <v>182.95614035089349</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -833,7 +833,7 @@
         <v>13</v>
       </c>
       <c r="C39">
-        <v>198.17165572366281</v>
+        <v>183.73508771927621</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -844,7 +844,7 @@
         <v>14</v>
       </c>
       <c r="C40">
-        <v>201.73987344181549</v>
+        <v>187.6210526316018</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -855,7 +855,7 @@
         <v>15</v>
       </c>
       <c r="C41">
-        <v>212.4400342563641</v>
+        <v>197.85087719301509</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -866,7 +866,7 @@
         <v>16</v>
       </c>
       <c r="C42">
-        <v>230.45805309731591</v>
+        <v>215.82280701748499</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -877,7 +877,7 @@
         <v>17</v>
       </c>
       <c r="C43">
-        <v>244.08902654867461</v>
+        <v>230.39649122807589</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -888,7 +888,7 @@
         <v>18</v>
       </c>
       <c r="C44">
-        <v>249.17203539822131</v>
+        <v>236.12280701755199</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -899,7 +899,7 @@
         <v>19</v>
       </c>
       <c r="C45">
-        <v>245.8559292035257</v>
+        <v>232.42678571424659</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -910,7 +910,7 @@
         <v>20</v>
       </c>
       <c r="C46">
-        <v>231.96457227142949</v>
+        <v>216.80877192988339</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -921,7 +921,7 @@
         <v>21</v>
       </c>
       <c r="C47">
-        <v>221.35834808257439</v>
+        <v>212.45964912278171</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -932,7 +932,7 @@
         <v>22</v>
       </c>
       <c r="C48">
-        <v>216.38112094395419</v>
+        <v>204.5438596491187</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -943,7 +943,7 @@
         <v>23</v>
       </c>
       <c r="C49">
-        <v>210.53812500001419</v>
+        <v>197.87321428571681</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -954,7 +954,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <v>189.62408602150481</v>
+        <v>178.89180327867169</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -965,7 +965,7 @@
         <v>1</v>
       </c>
       <c r="C51">
-        <v>192.1391666666581</v>
+        <v>180.0606557377042</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -976,7 +976,7 @@
         <v>2</v>
       </c>
       <c r="C52">
-        <v>197.68959677420679</v>
+        <v>184.5145161290495</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -987,7 +987,7 @@
         <v>3</v>
       </c>
       <c r="C53">
-        <v>216.53123655911361</v>
+        <v>203.74032258060609</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -998,7 +998,7 @@
         <v>4</v>
       </c>
       <c r="C54">
-        <v>226.9500268817346</v>
+        <v>207.8278688524743</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1009,7 +1009,7 @@
         <v>5</v>
       </c>
       <c r="C55">
-        <v>229.69413978491411</v>
+        <v>211.0344262294754</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1020,7 +1020,7 @@
         <v>6</v>
       </c>
       <c r="C56">
-        <v>217.48572580648241</v>
+        <v>200.70333333336751</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1031,7 +1031,7 @@
         <v>7</v>
       </c>
       <c r="C57">
-        <v>198.9392741935533</v>
+        <v>183.73220338984149</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1042,7 +1042,7 @@
         <v>8</v>
       </c>
       <c r="C58">
-        <v>185.24400537635341</v>
+        <v>171.63225806451541</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1053,7 +1053,7 @@
         <v>9</v>
       </c>
       <c r="C59">
-        <v>174.7181571815475</v>
+        <v>161.45573770489969</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1064,7 +1064,7 @@
         <v>10</v>
       </c>
       <c r="C60">
-        <v>167.5883114446732</v>
+        <v>155.46333333334579</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1075,7 +1075,7 @@
         <v>11</v>
       </c>
       <c r="C61">
-        <v>161.57386709889019</v>
+        <v>151.08709677417329</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1086,7 +1086,7 @@
         <v>12</v>
       </c>
       <c r="C62">
-        <v>155.59471644121811</v>
+        <v>147.87903225807949</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1097,7 +1097,7 @@
         <v>13</v>
       </c>
       <c r="C63">
-        <v>153.86255376340799</v>
+        <v>147.06129032253631</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1108,7 +1108,7 @@
         <v>14</v>
       </c>
       <c r="C64">
-        <v>156.51045698927939</v>
+        <v>148.7274193548665</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1119,7 +1119,7 @@
         <v>15</v>
       </c>
       <c r="C65">
-        <v>165.83376344085119</v>
+        <v>157.42903225804719</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1130,7 +1130,7 @@
         <v>16</v>
       </c>
       <c r="C66">
-        <v>180.2697043010717</v>
+        <v>171.40322580647791</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1141,7 +1141,7 @@
         <v>17</v>
       </c>
       <c r="C67">
-        <v>203.48564516129201</v>
+        <v>190.4524590163835</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1152,7 +1152,7 @@
         <v>18</v>
       </c>
       <c r="C68">
-        <v>213.45376344086441</v>
+        <v>200.78360655739311</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1163,7 +1163,7 @@
         <v>19</v>
       </c>
       <c r="C69">
-        <v>209.05809325176941</v>
+        <v>197.47166666665581</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1174,7 +1174,7 @@
         <v>20</v>
       </c>
       <c r="C70">
-        <v>195.83865406005941</v>
+        <v>185.34354838710499</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -1185,7 +1185,7 @@
         <v>21</v>
       </c>
       <c r="C71">
-        <v>185.54255376342641</v>
+        <v>179.2516129032048</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -1196,7 +1196,7 @@
         <v>22</v>
       </c>
       <c r="C72">
-        <v>182.90629032260179</v>
+        <v>175.62580645164749</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -1207,7 +1207,7 @@
         <v>23</v>
       </c>
       <c r="C73">
-        <v>180.97550135501751</v>
+        <v>172.9196721311491</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1218,7 +1218,7 @@
         <v>0</v>
       </c>
       <c r="C74">
-        <v>150.12418103450329</v>
+        <v>134.84237288138669</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -1229,7 +1229,7 @@
         <v>1</v>
       </c>
       <c r="C75">
-        <v>154.23511111110369</v>
+        <v>137.874576271188</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -1240,7 +1240,7 @@
         <v>2</v>
       </c>
       <c r="C76">
-        <v>168.12855555556021</v>
+        <v>148.58983050845561</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -1251,7 +1251,7 @@
         <v>3</v>
       </c>
       <c r="C77">
-        <v>183.21035931898609</v>
+        <v>162.72372881354269</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -1262,7 +1262,7 @@
         <v>4</v>
       </c>
       <c r="C78">
-        <v>186.6989499311361</v>
+        <v>166.14666666667131</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -1273,7 +1273,7 @@
         <v>5</v>
       </c>
       <c r="C79">
-        <v>173.63599630543229</v>
+        <v>152.02241379312429</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -1284,7 +1284,7 @@
         <v>6</v>
       </c>
       <c r="C80">
-        <v>162.06672222221289</v>
+        <v>142.39655172412989</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -1295,7 +1295,7 @@
         <v>7</v>
       </c>
       <c r="C81">
-        <v>152.95402777779569</v>
+        <v>136.15084745762161</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -1306,7 +1306,7 @@
         <v>8</v>
       </c>
       <c r="C82">
-        <v>144.94994444443441</v>
+        <v>129.32881355932841</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -1317,7 +1317,7 @@
         <v>9</v>
       </c>
       <c r="C83">
-        <v>140.3727499999863</v>
+        <v>124.9849999999938</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -1328,7 +1328,7 @@
         <v>10</v>
       </c>
       <c r="C84">
-        <v>136.0902222222231</v>
+        <v>121.7316666666341</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -1339,7 +1339,7 @@
         <v>11</v>
       </c>
       <c r="C85">
-        <v>130.35586111110749</v>
+        <v>116.70666666668841</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -1350,7 +1350,7 @@
         <v>12</v>
       </c>
       <c r="C86">
-        <v>128.61034126982361</v>
+        <v>115.87499999997669</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -1361,7 +1361,7 @@
         <v>13</v>
       </c>
       <c r="C87">
-        <v>128.53066141834131</v>
+        <v>115.8966666666868</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -1372,7 +1372,7 @@
         <v>14</v>
       </c>
       <c r="C88">
-        <v>131.0653862007195</v>
+        <v>117.07333333333951</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -1383,7 +1383,7 @@
         <v>15</v>
       </c>
       <c r="C89">
-        <v>137.27927777778049</v>
+        <v>121.5516666666682</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -1394,7 +1394,7 @@
         <v>16</v>
       </c>
       <c r="C90">
-        <v>151.21195788529491</v>
+        <v>136.1466666666519</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -1405,7 +1405,7 @@
         <v>17</v>
       </c>
       <c r="C91">
-        <v>167.39979211470441</v>
+        <v>150.63166666664961</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -1416,7 +1416,7 @@
         <v>18</v>
       </c>
       <c r="C92">
-        <v>174.18902777778371</v>
+        <v>158.2116666667047</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -1427,7 +1427,7 @@
         <v>19</v>
       </c>
       <c r="C93">
-        <v>165.79933333333369</v>
+        <v>151.48833333333411</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -1438,7 +1438,7 @@
         <v>20</v>
       </c>
       <c r="C94">
-        <v>152.0766388888878</v>
+        <v>139.70666666665349</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -1449,7 +1449,7 @@
         <v>21</v>
       </c>
       <c r="C95">
-        <v>145.48780555555709</v>
+        <v>132.55084745764691</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -1460,7 +1460,7 @@
         <v>22</v>
       </c>
       <c r="C96">
-        <v>144.90436111113911</v>
+        <v>131.01034482759991</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -1471,7 +1471,7 @@
         <v>23</v>
       </c>
       <c r="C97">
-        <v>147.52987452104671</v>
+        <v>132.0586206896335</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -1482,7 +1482,7 @@
         <v>0</v>
       </c>
       <c r="C98">
-        <v>82.70682795697283</v>
+        <v>74.524999999980594</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -1493,7 +1493,7 @@
         <v>1</v>
       </c>
       <c r="C99">
-        <v>83.968790322596647</v>
+        <v>76.293103448311996</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -1504,7 +1504,7 @@
         <v>2</v>
       </c>
       <c r="C100">
-        <v>90.323709677413831</v>
+        <v>82.786885245882559</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -1515,7 +1515,7 @@
         <v>3</v>
       </c>
       <c r="C101">
-        <v>100.3655376343917</v>
+        <v>93.777419354826691</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -1526,7 +1526,7 @@
         <v>4</v>
       </c>
       <c r="C102">
-        <v>97.901236559145133</v>
+        <v>90.361290322612945</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -1537,7 +1537,7 @@
         <v>5</v>
       </c>
       <c r="C103">
-        <v>88.838844086051054</v>
+        <v>81.170967741955764</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -1548,7 +1548,7 @@
         <v>6</v>
       </c>
       <c r="C104">
-        <v>85.648790322551164</v>
+        <v>79.019354838678879</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -1559,7 +1559,7 @@
         <v>7</v>
       </c>
       <c r="C105">
-        <v>85.127365591410069</v>
+        <v>79.532258064538667</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -1570,7 +1570,7 @@
         <v>8</v>
       </c>
       <c r="C106">
-        <v>82.930913978505075</v>
+        <v>77.838709677415594</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -1581,7 +1581,7 @@
         <v>9</v>
       </c>
       <c r="C107">
-        <v>82.792607526869446</v>
+        <v>77.822580645135005</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -1592,7 +1592,7 @@
         <v>10</v>
       </c>
       <c r="C108">
-        <v>81.846075268790898</v>
+        <v>76.945161290305307</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -1603,7 +1603,7 @@
         <v>11</v>
       </c>
       <c r="C109">
-        <v>79.862956989281471</v>
+        <v>74.611290322627966</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -1614,7 +1614,7 @@
         <v>12</v>
       </c>
       <c r="C110">
-        <v>77.784139784935476</v>
+        <v>72.206451612881452</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -1625,7 +1625,7 @@
         <v>13</v>
       </c>
       <c r="C111">
-        <v>76.688145161290919</v>
+        <v>70.732258064525894</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -1636,7 +1636,7 @@
         <v>14</v>
       </c>
       <c r="C112">
-        <v>77.967258064541966</v>
+        <v>72.27096774197004</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -1647,7 +1647,7 @@
         <v>15</v>
       </c>
       <c r="C113">
-        <v>82.208172042977111</v>
+        <v>75.883870967682597</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -1658,7 +1658,7 @@
         <v>16</v>
       </c>
       <c r="C114">
-        <v>90.338091397857966</v>
+        <v>82.851612903237822</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -1669,7 +1669,7 @@
         <v>17</v>
       </c>
       <c r="C115">
-        <v>100.0174462365507</v>
+        <v>92.749999999996248</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -1680,7 +1680,7 @@
         <v>18</v>
       </c>
       <c r="C116">
-        <v>104.7540860214973</v>
+        <v>96.253225806443353</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -1691,7 +1691,7 @@
         <v>19</v>
       </c>
       <c r="C117">
-        <v>99.101559139818193</v>
+        <v>89.896774193598702</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -1702,7 +1702,7 @@
         <v>20</v>
       </c>
       <c r="C118">
-        <v>89.588145161286036</v>
+        <v>81.05645161287319</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -1713,7 +1713,7 @@
         <v>21</v>
       </c>
       <c r="C119">
-        <v>80.888629032231322</v>
+        <v>72.441935483850685</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -1724,7 +1724,7 @@
         <v>22</v>
       </c>
       <c r="C120">
-        <v>80.316129032285858</v>
+        <v>72.716129032282851</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -1735,7 +1735,7 @@
         <v>23</v>
       </c>
       <c r="C121">
-        <v>80.668010752678157</v>
+        <v>73.109677419336819</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -1746,7 +1746,7 @@
         <v>0</v>
       </c>
       <c r="C122">
-        <v>38.287316384224091</v>
+        <v>39.82666666670314</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -1757,7 +1757,7 @@
         <v>1</v>
       </c>
       <c r="C123">
-        <v>38.890225988680541</v>
+        <v>40.456666666661228</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -1768,7 +1768,7 @@
         <v>2</v>
       </c>
       <c r="C124">
-        <v>40.780903954805723</v>
+        <v>41.98666666666977</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -1779,7 +1779,7 @@
         <v>3</v>
       </c>
       <c r="C125">
-        <v>48.51016949154377</v>
+        <v>49.951666666672097</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -1790,7 +1790,7 @@
         <v>4</v>
       </c>
       <c r="C126">
-        <v>50.712485875671938</v>
+        <v>51.639999999979047</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -1801,7 +1801,7 @@
         <v>5</v>
       </c>
       <c r="C127">
-        <v>49.572203389845463</v>
+        <v>50.65500000002406</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -1812,7 +1812,7 @@
         <v>6</v>
       </c>
       <c r="C128">
-        <v>48.784802259886213</v>
+        <v>50.887931034470718</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -1823,7 +1823,7 @@
         <v>7</v>
       </c>
       <c r="C129">
-        <v>50.294901960769067</v>
+        <v>52.617241379275022</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -1834,7 +1834,7 @@
         <v>8</v>
       </c>
       <c r="C130">
-        <v>49.502661064417808</v>
+        <v>51.359322033897513</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -1845,7 +1845,7 @@
         <v>9</v>
       </c>
       <c r="C131">
-        <v>50.357002801128793</v>
+        <v>51.466666666666669</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -1856,7 +1856,7 @@
         <v>10</v>
       </c>
       <c r="C132">
-        <v>50.463473389374222</v>
+        <v>52.616949152584198</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -1867,7 +1867,7 @@
         <v>11</v>
       </c>
       <c r="C133">
-        <v>48.732352941163953</v>
+        <v>50.889830508450899</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -1878,7 +1878,7 @@
         <v>12</v>
       </c>
       <c r="C134">
-        <v>47.672231638449901</v>
+        <v>48.995000000010869</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -1889,7 +1889,7 @@
         <v>13</v>
       </c>
       <c r="C135">
-        <v>47.014632768327203</v>
+        <v>47.924999999988358</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -1900,7 +1900,7 @@
         <v>14</v>
       </c>
       <c r="C136">
-        <v>46.774689265547551</v>
+        <v>48.545762711887292</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -1911,7 +1911,7 @@
         <v>15</v>
       </c>
       <c r="C137">
-        <v>48.796441589214773</v>
+        <v>49.708474576271968</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -1922,7 +1922,7 @@
         <v>16</v>
       </c>
       <c r="C138">
-        <v>53.827004738471679</v>
+        <v>53.866666666662788</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -1933,7 +1933,7 @@
         <v>17</v>
       </c>
       <c r="C139">
-        <v>60.578983050848997</v>
+        <v>60.053333333313162</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -1944,7 +1944,7 @@
         <v>18</v>
       </c>
       <c r="C140">
-        <v>61.885338983043702</v>
+        <v>61.253333333324797</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -1955,7 +1955,7 @@
         <v>19</v>
       </c>
       <c r="C141">
-        <v>54.769073264066613</v>
+        <v>54.754999999993018</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -1966,7 +1966,7 @@
         <v>20</v>
       </c>
       <c r="C142">
-        <v>47.737367413894638</v>
+        <v>48.173333333362827</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -1977,7 +1977,7 @@
         <v>21</v>
       </c>
       <c r="C143">
-        <v>39.563615819204493</v>
+        <v>41.336666666658132</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -1988,7 +1988,7 @@
         <v>22</v>
       </c>
       <c r="C144">
-        <v>39.120508474579978</v>
+        <v>41.508333333321687</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -1999,7 +1999,7 @@
         <v>23</v>
       </c>
       <c r="C145">
-        <v>38.370112994341447</v>
+        <v>41.113333333334111</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -2010,7 +2010,7 @@
         <v>0</v>
       </c>
       <c r="C146">
-        <v>34.286396396391488</v>
+        <v>31.17580645163018</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -2021,7 +2021,7 @@
         <v>1</v>
       </c>
       <c r="C147">
-        <v>34.416666666632047</v>
+        <v>30.762903225750868</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -2032,7 +2032,7 @@
         <v>2</v>
       </c>
       <c r="C148">
-        <v>35.399026548710403</v>
+        <v>32.50645161293928</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -2043,7 +2043,7 @@
         <v>3</v>
       </c>
       <c r="C149">
-        <v>42.178141592922458</v>
+        <v>38.680327868856267</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -2054,7 +2054,7 @@
         <v>4</v>
       </c>
       <c r="C150">
-        <v>43.153008849569183</v>
+        <v>39.100000000006759</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -2065,7 +2065,7 @@
         <v>5</v>
       </c>
       <c r="C151">
-        <v>41.569616519138258</v>
+        <v>37.598387096741902</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -2076,7 +2076,7 @@
         <v>6</v>
       </c>
       <c r="C152">
-        <v>41.958584070788802</v>
+        <v>39.142372881342517</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -2087,7 +2087,7 @@
         <v>7</v>
       </c>
       <c r="C153">
-        <v>46.530117994137271</v>
+        <v>39.821666666714009</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -2098,7 +2098,7 @@
         <v>8</v>
       </c>
       <c r="C154">
-        <v>43.816578171071718</v>
+        <v>38.299999999978333</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -2109,7 +2109,7 @@
         <v>9</v>
       </c>
       <c r="C155">
-        <v>44.29471976403147</v>
+        <v>39.310000000005431</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -2120,7 +2120,7 @@
         <v>10</v>
       </c>
       <c r="C156">
-        <v>43.165604719736578</v>
+        <v>37.043548387069727</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -2131,7 +2131,7 @@
         <v>11</v>
       </c>
       <c r="C157">
-        <v>41.652172619049708</v>
+        <v>35.579032258081789</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -2142,7 +2142,7 @@
         <v>12</v>
       </c>
       <c r="C158">
-        <v>40.958214285699277</v>
+        <v>35.012903225773407</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -2153,7 +2153,7 @@
         <v>13</v>
       </c>
       <c r="C159">
-        <v>40.851428571458591</v>
+        <v>34.468333333381452</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -2164,7 +2164,7 @@
         <v>14</v>
       </c>
       <c r="C160">
-        <v>40.410565476191032</v>
+        <v>34.103278688513903</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -2175,7 +2175,7 @@
         <v>15</v>
       </c>
       <c r="C161">
-        <v>41.674985250734217</v>
+        <v>36.521311475402968</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -2186,7 +2186,7 @@
         <v>16</v>
       </c>
       <c r="C162">
-        <v>45.203157894751428</v>
+        <v>39.88387096776146</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -2197,7 +2197,7 @@
         <v>17</v>
       </c>
       <c r="C163">
-        <v>49.826405797088917</v>
+        <v>44.323333333331782</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -2208,7 +2208,7 @@
         <v>18</v>
       </c>
       <c r="C164">
-        <v>50.949739130435553</v>
+        <v>47.540983606549737</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -2219,7 +2219,7 @@
         <v>19</v>
       </c>
       <c r="C165">
-        <v>47.382138535991032</v>
+        <v>43.559677419354088</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -2230,7 +2230,7 @@
         <v>20</v>
       </c>
       <c r="C166">
-        <v>41.428963482858968</v>
+        <v>37.855737704932537</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -2241,7 +2241,7 @@
         <v>21</v>
       </c>
       <c r="C167">
-        <v>34.031160714291858</v>
+        <v>31.193333333338771</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -2252,7 +2252,7 @@
         <v>22</v>
       </c>
       <c r="C168">
-        <v>34.512142857114668</v>
+        <v>30.926229508147099</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -2263,7 +2263,7 @@
         <v>23</v>
       </c>
       <c r="C169">
-        <v>34.598727272755717</v>
+        <v>30.991803278719061</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -2274,7 +2274,7 @@
         <v>0</v>
       </c>
       <c r="C170">
-        <v>35.002672955974766</v>
+        <v>29.56885245904617</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -2285,7 +2285,7 @@
         <v>1</v>
       </c>
       <c r="C171">
-        <v>35.643679245276253</v>
+        <v>31.179661016938891</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -2296,7 +2296,7 @@
         <v>2</v>
       </c>
       <c r="C172">
-        <v>36.695919003135252</v>
+        <v>31.485483870976751</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -2307,7 +2307,7 @@
         <v>3</v>
       </c>
       <c r="C173">
-        <v>42.432716049373589</v>
+        <v>33.880327868836432</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -2318,7 +2318,7 @@
         <v>4</v>
       </c>
       <c r="C174">
-        <v>45.356352201252207</v>
+        <v>36.062295081960343</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -2329,7 +2329,7 @@
         <v>5</v>
       </c>
       <c r="C175">
-        <v>44.328285714298751</v>
+        <v>35.900000000021372</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -2340,7 +2340,7 @@
         <v>6</v>
       </c>
       <c r="C176">
-        <v>44.869182389937912</v>
+        <v>36.279999999973612</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -2351,7 +2351,7 @@
         <v>7</v>
       </c>
       <c r="C177">
-        <v>44.855943396216347</v>
+        <v>35.515789473694831</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -2362,7 +2362,7 @@
         <v>8</v>
       </c>
       <c r="C178">
-        <v>44.428480725642302</v>
+        <v>35.989285714308998</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -2373,7 +2373,7 @@
         <v>9</v>
       </c>
       <c r="C179">
-        <v>44.251632756550293</v>
+        <v>36.550877192956307</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -2384,7 +2384,7 @@
         <v>10</v>
       </c>
       <c r="C180">
-        <v>43.692551865385447</v>
+        <v>35.21999999997206</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -2395,7 +2395,7 @@
         <v>11</v>
       </c>
       <c r="C181">
-        <v>45.200398467434567</v>
+        <v>36.053333333351958</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -2406,7 +2406,7 @@
         <v>12</v>
       </c>
       <c r="C182">
-        <v>42.089496855343967</v>
+        <v>34.762903225803448</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -2417,7 +2417,7 @@
         <v>13</v>
       </c>
       <c r="C183">
-        <v>41.744528301894867</v>
+        <v>33.25000000001878</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -2428,7 +2428,7 @@
         <v>14</v>
       </c>
       <c r="C184">
-        <v>41.022672955949467</v>
+        <v>33.736065573726982</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
@@ -2439,7 +2439,7 @@
         <v>15</v>
       </c>
       <c r="C185">
-        <v>41.70910838976063</v>
+        <v>35.088524590204393</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
@@ -2450,7 +2450,7 @@
         <v>16</v>
       </c>
       <c r="C186">
-        <v>44.618669646646588</v>
+        <v>37.336065573759043</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
@@ -2461,7 +2461,7 @@
         <v>17</v>
       </c>
       <c r="C187">
-        <v>49.098842541109427</v>
+        <v>39.833870967752453</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -2472,7 +2472,7 @@
         <v>18</v>
       </c>
       <c r="C188">
-        <v>51.074898000192938</v>
+        <v>41.149999999993241</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
@@ -2483,7 +2483,7 @@
         <v>19</v>
       </c>
       <c r="C189">
-        <v>47.108722741435997</v>
+        <v>38.359677419366847</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
@@ -2494,7 +2494,7 @@
         <v>20</v>
       </c>
       <c r="C190">
-        <v>41.333553459117503</v>
+        <v>33.977049180298863</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
@@ -2505,7 +2505,7 @@
         <v>21</v>
       </c>
       <c r="C191">
-        <v>33.827999999981728</v>
+        <v>28.71000000000155</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
@@ -2516,7 +2516,7 @@
         <v>22</v>
       </c>
       <c r="C192">
-        <v>33.41261682242795</v>
+        <v>28.647540983602742</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
@@ -2527,7 +2527,7 @@
         <v>23</v>
       </c>
       <c r="C193">
-        <v>34.311775700949681</v>
+        <v>30.329508196730469</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
@@ -2538,7 +2538,7 @@
         <v>0</v>
       </c>
       <c r="C194">
-        <v>53.751960784310327</v>
+        <v>48.476666666656577</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -2549,7 +2549,7 @@
         <v>1</v>
       </c>
       <c r="C195">
-        <v>55.277338935608171</v>
+        <v>49.890000000045013</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -2560,7 +2560,7 @@
         <v>2</v>
       </c>
       <c r="C196">
-        <v>59.827591036403348</v>
+        <v>53.993333333299958</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -2571,7 +2571,7 @@
         <v>3</v>
       </c>
       <c r="C197">
-        <v>69.440252100834584</v>
+        <v>63.752542372883717</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -2582,7 +2582,7 @@
         <v>4</v>
       </c>
       <c r="C198">
-        <v>72.268431372551191</v>
+        <v>66.359322033913301</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -2593,7 +2593,7 @@
         <v>5</v>
       </c>
       <c r="C199">
-        <v>72.350444444438708</v>
+        <v>65.038333333330229</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
@@ -2604,7 +2604,7 @@
         <v>6</v>
       </c>
       <c r="C200">
-        <v>70.717622222242056</v>
+        <v>63.956666666676753</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
@@ -2615,7 +2615,7 @@
         <v>7</v>
       </c>
       <c r="C201">
-        <v>70.785877777774786</v>
+        <v>65.113333333353509</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
@@ -2626,7 +2626,7 @@
         <v>8</v>
       </c>
       <c r="C202">
-        <v>68.681055555569273</v>
+        <v>64.188333333330235</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
@@ -2637,7 +2637,7 @@
         <v>9</v>
       </c>
       <c r="C203">
-        <v>67.333999999989956</v>
+        <v>62.829999999977503</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
@@ -2648,7 +2648,7 @@
         <v>10</v>
       </c>
       <c r="C204">
-        <v>66.723138888894269</v>
+        <v>62.338333333349631</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
@@ -2659,7 +2659,7 @@
         <v>11</v>
       </c>
       <c r="C205">
-        <v>64.898527777775115</v>
+        <v>61.031666666665117</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
@@ -2670,7 +2670,7 @@
         <v>12</v>
       </c>
       <c r="C206">
-        <v>62.966333333324293</v>
+        <v>58.4266666666527</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
@@ -2681,7 +2681,7 @@
         <v>13</v>
       </c>
       <c r="C207">
-        <v>62.585166666670311</v>
+        <v>57.153333333355839</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
@@ -2692,7 +2692,7 @@
         <v>14</v>
       </c>
       <c r="C208">
-        <v>64.280999999992005</v>
+        <v>58.586666666642607</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
@@ -2703,7 +2703,7 @@
         <v>15</v>
       </c>
       <c r="C209">
-        <v>67.26058333332476</v>
+        <v>60.545000000010873</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
@@ -2714,7 +2714,7 @@
         <v>16</v>
       </c>
       <c r="C210">
-        <v>76.165194444438868</v>
+        <v>68.708333333306172</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
@@ -2725,7 +2725,7 @@
         <v>17</v>
       </c>
       <c r="C211">
-        <v>86.226653225819845</v>
+        <v>75.843333333346521</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
@@ -2736,7 +2736,7 @@
         <v>18</v>
       </c>
       <c r="C212">
-        <v>84.448235663075081</v>
+        <v>74.604999999989133</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
@@ -2747,7 +2747,7 @@
         <v>19</v>
       </c>
       <c r="C213">
-        <v>73.987249999998795</v>
+        <v>65.131666666661232</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
@@ -2758,7 +2758,7 @@
         <v>20</v>
       </c>
       <c r="C214">
-        <v>63.735027777789703</v>
+        <v>56.206666666672866</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
@@ -2769,7 +2769,7 @@
         <v>21</v>
       </c>
       <c r="C215">
-        <v>57.02058823527905</v>
+        <v>48.973333333324021</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
@@ -2780,7 +2780,7 @@
         <v>22</v>
       </c>
       <c r="C216">
-        <v>56.835070028007927</v>
+        <v>48.821666666671327</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
@@ -2791,7 +2791,7 @@
         <v>23</v>
       </c>
       <c r="C217">
-        <v>56.519887955179399</v>
+        <v>49.313333333326348</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
@@ -2802,7 +2802,7 @@
         <v>0</v>
       </c>
       <c r="C218">
-        <v>117.9368010752904</v>
+        <v>109.97580645165419</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
@@ -2813,7 +2813,7 @@
         <v>1</v>
       </c>
       <c r="C219">
-        <v>120.5366397849369</v>
+        <v>112.52419354837581</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
@@ -2824,7 +2824,7 @@
         <v>2</v>
       </c>
       <c r="C220">
-        <v>130.57631720430331</v>
+        <v>123.49836065573621</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
@@ -2835,7 +2835,7 @@
         <v>3</v>
       </c>
       <c r="C221">
-        <v>145.85182795700359</v>
+        <v>137.57419354837731</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
@@ -2846,7 +2846,7 @@
         <v>4</v>
       </c>
       <c r="C222">
-        <v>149.33965053762901</v>
+        <v>142.06774193549811</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
@@ -2857,7 +2857,7 @@
         <v>5</v>
       </c>
       <c r="C223">
-        <v>147.27908602150649</v>
+        <v>142.10833333332559</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
@@ -2868,7 +2868,7 @@
         <v>6</v>
       </c>
       <c r="C224">
-        <v>143.72010752687979</v>
+        <v>138.93442622950059</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
@@ -2879,7 +2879,7 @@
         <v>7</v>
       </c>
       <c r="C225">
-        <v>131.83190860215859</v>
+        <v>130.92786885247199</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
@@ -2890,7 +2890,7 @@
         <v>8</v>
       </c>
       <c r="C226">
-        <v>122.9297432332035</v>
+        <v>125.2933333333155</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
@@ -2901,7 +2901,7 @@
         <v>9</v>
       </c>
       <c r="C227">
-        <v>116.370699014449</v>
+        <v>116.7000000000323</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
@@ -2912,7 +2912,7 @@
         <v>10</v>
       </c>
       <c r="C228">
-        <v>111.4128910856774</v>
+        <v>111.4387096773998</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
@@ -2923,7 +2923,7 @@
         <v>11</v>
       </c>
       <c r="C229">
-        <v>106.5594768403643</v>
+        <v>107.348387096802</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
@@ -2934,7 +2934,7 @@
         <v>12</v>
       </c>
       <c r="C230">
-        <v>105.7545822994293</v>
+        <v>108.1677419354636</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
@@ -2945,7 +2945,7 @@
         <v>13</v>
       </c>
       <c r="C231">
-        <v>107.72157181571311</v>
+        <v>109.2483870967727</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
@@ -2956,7 +2956,7 @@
         <v>14</v>
       </c>
       <c r="C232">
-        <v>111.8085365853683</v>
+        <v>112.72903225807499</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
@@ -2967,7 +2967,7 @@
         <v>15</v>
       </c>
       <c r="C233">
-        <v>124.3575806451469</v>
+        <v>122.6606557376942</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
@@ -2978,7 +2978,7 @@
         <v>16</v>
       </c>
       <c r="C234">
-        <v>140.4509677419471</v>
+        <v>135.4322580645094</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
@@ -2989,7 +2989,7 @@
         <v>17</v>
       </c>
       <c r="C235">
-        <v>150.38469377565079</v>
+        <v>142.81774193549811</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
@@ -3000,7 +3000,7 @@
         <v>18</v>
       </c>
       <c r="C236">
-        <v>146.31970138563361</v>
+        <v>138.5112903225874</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
@@ -3011,7 +3011,7 @@
         <v>19</v>
       </c>
       <c r="C237">
-        <v>138.00245794310561</v>
+        <v>129.6290322580457</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
@@ -3022,7 +3022,7 @@
         <v>20</v>
       </c>
       <c r="C238">
-        <v>125.12010926119009</v>
+        <v>117.83387096774869</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
@@ -3033,7 +3033,7 @@
         <v>21</v>
       </c>
       <c r="C239">
-        <v>116.8152956989492</v>
+        <v>108.14193548387919</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
@@ -3044,7 +3044,7 @@
         <v>22</v>
       </c>
       <c r="C240">
-        <v>115.68099462364199</v>
+        <v>106.706451612904</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
@@ -3055,7 +3055,7 @@
         <v>23</v>
       </c>
       <c r="C241">
-        <v>117.66163978491809</v>
+        <v>109.17580645157381</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
@@ -3066,7 +3066,7 @@
         <v>0</v>
       </c>
       <c r="C242">
-        <v>175.92279211470739</v>
+        <v>181.06610169492549</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
@@ -3077,7 +3077,7 @@
         <v>1</v>
       </c>
       <c r="C243">
-        <v>178.29723566307709</v>
+        <v>184.30677966102641</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
@@ -3088,7 +3088,7 @@
         <v>2</v>
       </c>
       <c r="C244">
-        <v>181.08730555553919</v>
+        <v>187.1610169491328</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
@@ -3099,7 +3099,7 @@
         <v>3</v>
       </c>
       <c r="C245">
-        <v>201.5233333333376</v>
+        <v>212.0949152542191</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
@@ -3110,7 +3110,7 @@
         <v>4</v>
       </c>
       <c r="C246">
-        <v>210.66769444445569</v>
+        <v>219.36166666670471</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
@@ -3121,7 +3121,7 @@
         <v>5</v>
       </c>
       <c r="C247">
-        <v>214.33924999999391</v>
+        <v>223.56666666665501</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
@@ -3132,7 +3132,7 @@
         <v>6</v>
       </c>
       <c r="C248">
-        <v>215.84023467431149</v>
+        <v>224.0916666666279</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
@@ -3143,7 +3143,7 @@
         <v>7</v>
       </c>
       <c r="C249">
-        <v>211.38323754790471</v>
+        <v>218.394915254246</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
@@ -3154,7 +3154,7 @@
         <v>8</v>
       </c>
       <c r="C250">
-        <v>199.42775000000739</v>
+        <v>205.45862068966079</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
@@ -3165,7 +3165,7 @@
         <v>9</v>
       </c>
       <c r="C251">
-        <v>191.1512729885163</v>
+        <v>197.433333333376</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
@@ -3176,7 +3176,7 @@
         <v>10</v>
       </c>
       <c r="C252">
-        <v>186.24525478925591</v>
+        <v>191.93833333331469</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
@@ -3187,7 +3187,7 @@
         <v>11</v>
       </c>
       <c r="C253">
-        <v>180.5506851852154</v>
+        <v>185.04166666670159</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
@@ -3198,7 +3198,7 @@
         <v>12</v>
       </c>
       <c r="C254">
-        <v>179.4938981481294</v>
+        <v>183.66833333330379</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
@@ -3209,7 +3209,7 @@
         <v>13</v>
       </c>
       <c r="C255">
-        <v>180.60016666666971</v>
+        <v>185.47833333333261</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
@@ -3220,7 +3220,7 @@
         <v>14</v>
       </c>
       <c r="C256">
-        <v>186.11391666664471</v>
+        <v>190.9983333333046</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
@@ -3231,7 +3231,7 @@
         <v>15</v>
       </c>
       <c r="C257">
-        <v>197.13427777776769</v>
+        <v>202.92166666666739</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
@@ -3242,7 +3242,7 @@
         <v>16</v>
       </c>
       <c r="C258">
-        <v>205.5893333333506</v>
+        <v>211.63333333334501</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
@@ -3253,7 +3253,7 @@
         <v>17</v>
       </c>
       <c r="C259">
-        <v>210.27463888890239</v>
+        <v>214.0733333333512</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
@@ -3264,7 +3264,7 @@
         <v>18</v>
       </c>
       <c r="C260">
-        <v>214.92969444444651</v>
+        <v>217.7566666667</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
@@ -3275,7 +3275,7 @@
         <v>19</v>
       </c>
       <c r="C261">
-        <v>210.64105555555139</v>
+        <v>211.97833333330539</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
@@ -3286,7 +3286,7 @@
         <v>20</v>
       </c>
       <c r="C262">
-        <v>193.2999444444159</v>
+        <v>197.3186440677579</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
@@ -3297,7 +3297,7 @@
         <v>21</v>
       </c>
       <c r="C263">
-        <v>184.47705555557431</v>
+        <v>189.33898305087109</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
@@ -3308,7 +3308,7 @@
         <v>22</v>
       </c>
       <c r="C264">
-        <v>179.5510555555646</v>
+        <v>184.09152542372331</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
@@ -3319,7 +3319,7 @@
         <v>23</v>
       </c>
       <c r="C265">
-        <v>175.08044444443951</v>
+        <v>178.6316666666612</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
@@ -3330,7 +3330,7 @@
         <v>0</v>
       </c>
       <c r="C266">
-        <v>216.61991935481521</v>
+        <v>212.2838709677284</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
@@ -3341,7 +3341,7 @@
         <v>1</v>
       </c>
       <c r="C267">
-        <v>218.62024193547941</v>
+        <v>215.1032258064651</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
@@ -3352,7 +3352,7 @@
         <v>2</v>
       </c>
       <c r="C268">
-        <v>222.23088709678271</v>
+        <v>219.70483870966919</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
@@ -3363,7 +3363,7 @@
         <v>3</v>
       </c>
       <c r="C269">
-        <v>243.95008064516361</v>
+        <v>243.9096774193421</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
@@ -3374,7 +3374,7 @@
         <v>4</v>
       </c>
       <c r="C270">
-        <v>250.95080645161781</v>
+        <v>251.0274193548567</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
@@ -3385,7 +3385,7 @@
         <v>5</v>
       </c>
       <c r="C271">
-        <v>252.28852150537969</v>
+        <v>252.42741935483119</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
@@ -3396,7 +3396,7 @@
         <v>6</v>
       </c>
       <c r="C272">
-        <v>255.40529359221239</v>
+        <v>254.61612903225361</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
@@ -3407,7 +3407,7 @@
         <v>7</v>
       </c>
       <c r="C273">
-        <v>260.90599759750728</v>
+        <v>259.84098360655821</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
@@ -3418,7 +3418,7 @@
         <v>8</v>
       </c>
       <c r="C274">
-        <v>253.12293901554341</v>
+        <v>253.41785714283051</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
@@ -3429,7 +3429,7 @@
         <v>9</v>
       </c>
       <c r="C275">
-        <v>240.20804655959361</v>
+        <v>240.52419354838341</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
@@ -3440,7 +3440,7 @@
         <v>10</v>
       </c>
       <c r="C276">
-        <v>233.54963183728981</v>
+        <v>233.1338709677502</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
@@ -3451,7 +3451,7 @@
         <v>11</v>
       </c>
       <c r="C277">
-        <v>227.7708064516041</v>
+        <v>227.6822580645244</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
@@ -3462,7 +3462,7 @@
         <v>12</v>
       </c>
       <c r="C278">
-        <v>225.0039516129182</v>
+        <v>223.95483870969551</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
@@ -3473,7 +3473,7 @@
         <v>13</v>
       </c>
       <c r="C279">
-        <v>226.58261424733041</v>
+        <v>224.55322580646359</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
@@ -3484,7 +3484,7 @@
         <v>14</v>
       </c>
       <c r="C280">
-        <v>232.70633736557531</v>
+        <v>230.03064516129629</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
@@ -3495,7 +3495,7 @@
         <v>15</v>
       </c>
       <c r="C281">
-        <v>241.16263440859339</v>
+        <v>239.40967741933079</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
@@ -3506,7 +3506,7 @@
         <v>16</v>
       </c>
       <c r="C282">
-        <v>243.91481182795019</v>
+        <v>241.83870967737431</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
@@ -3517,7 +3517,7 @@
         <v>17</v>
       </c>
       <c r="C283">
-        <v>247.07010752688569</v>
+        <v>243.71451612906679</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
@@ -3528,7 +3528,7 @@
         <v>18</v>
       </c>
       <c r="C284">
-        <v>251.93698924731069</v>
+        <v>247.97096774188589</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
@@ -3539,7 +3539,7 @@
         <v>19</v>
       </c>
       <c r="C285">
-        <v>248.5978494623578</v>
+        <v>243.60806451619209</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
@@ -3550,7 +3550,7 @@
         <v>20</v>
       </c>
       <c r="C286">
-        <v>234.1700806451864</v>
+        <v>228.97258064516211</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
@@ -3561,7 +3561,7 @@
         <v>21</v>
       </c>
       <c r="C287">
-        <v>224.3923924731038</v>
+        <v>221.38709677415969</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
@@ -3572,7 +3572,7 @@
         <v>22</v>
       </c>
       <c r="C288">
-        <v>218.8363440860262</v>
+        <v>215.2564516129205</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
@@ -3583,7 +3583,7 @@
         <v>23</v>
       </c>
       <c r="C289">
-        <v>212.68435483872361</v>
+        <v>209.8032258064824</v>
       </c>
     </row>
   </sheetData>

</xml_diff>